<commit_message>
debug with ID3 and update dataset
</commit_message>
<xml_diff>
--- a/Decision_Tree/ID3/data/lenses.xlsx
+++ b/Decision_Tree/ID3/data/lenses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Blog\Machine_Learning\Decision_Tree\ID3\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C582297-B7F2-4BD6-99E3-33FE05A74526}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C58B13EF-A5E3-41D1-B658-E0F8871DFC9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11592" yWindow="264" windowWidth="14472" windowHeight="11940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="15">
   <si>
     <t>age</t>
   </si>
@@ -38,10 +38,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>prescription</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>astigmatic</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -58,15 +54,9 @@
     <t>young</t>
   </si>
   <si>
-    <t>pre-presbyopic</t>
-  </si>
-  <si>
     <t>presbyopic</t>
   </si>
   <si>
-    <t>hypermetrope</t>
-  </si>
-  <si>
     <t>myope</t>
   </si>
   <si>
@@ -77,6 +67,12 @@
   </si>
   <si>
     <t>normal</t>
+  </si>
+  <si>
+    <t>hyper</t>
+  </si>
+  <si>
+    <t>pre</t>
   </si>
 </sst>
 </file>
@@ -407,12 +403,12 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="29.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="22.44140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="12" style="1" customWidth="1"/>
     <col min="4" max="4" width="19.21875" style="1" customWidth="1"/>
@@ -424,10 +420,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -438,410 +434,410 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>